<commit_message>
abrindo turmas de pacotes e visualizacao
</commit_message>
<xml_diff>
--- a/inst/pacotes.xlsx
+++ b/inst/pacotes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/curso-r/site-v2/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F5B7E1-D85D-9F45-9735-8E7EBFC78737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93FCB26-0A61-244E-AEEB-9035E54E4B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="460" windowWidth="24880" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>pacote</t>
   </si>
@@ -254,6 +254,33 @@
   </si>
   <si>
     <t>Transforme seu script R em uma API.</t>
+  </si>
+  <si>
+    <t>pkgdown</t>
+  </si>
+  <si>
+    <t>Seus pacotes maravilhosamente documentados.</t>
+  </si>
+  <si>
+    <t>https://pkgdown.r-lib.org/</t>
+  </si>
+  <si>
+    <t>testthat</t>
+  </si>
+  <si>
+    <t>https://testthat.r-lib.org/</t>
+  </si>
+  <si>
+    <t>Teste.</t>
+  </si>
+  <si>
+    <t>https://r-spatial.github.io/sf/</t>
+  </si>
+  <si>
+    <t>Simplificando dados espaciais.</t>
+  </si>
+  <si>
+    <t>sf</t>
   </si>
 </sst>
 </file>
@@ -652,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -952,7 +979,37 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="3"/>
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>